<commit_message>
Updated sentence correction notes
</commit_message>
<xml_diff>
--- a/gmat/verbal/SC_Error_Log.xlsx
+++ b/gmat/verbal/SC_Error_Log.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GPruthi\Documents\algorithms\gmat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="32">
   <si>
     <t>Slow</t>
   </si>
@@ -111,12 +106,24 @@
   <si>
     <t>Missed the dot and thought that sentence is incomplete</t>
   </si>
+  <si>
+    <t>meaning problem, cause-
+effect  idntification connection problem</t>
+  </si>
+  <si>
+    <t>which always refers to the attached noun</t>
+  </si>
+  <si>
+    <t>If the part of speech which follows comma is not participle then that 
+modifies the preceding noun. The far off modifier cannot be the primary 
+mistake in the sentence</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,6 +163,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -301,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,6 +361,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -689,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -699,9 +725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I199" sqref="I199"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M178" sqref="M178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2816,7 +2842,9 @@
       <c r="E73" s="8"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
-      <c r="H73" s="10"/>
+      <c r="H73" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="I73" s="10" t="s">
         <v>11</v>
       </c>
@@ -3002,7 +3030,9 @@
       <c r="E79" s="8"/>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
+      <c r="H79" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="I79" s="10" t="s">
         <v>11</v>
       </c>
@@ -3217,7 +3247,9 @@
       <c r="E86" s="8"/>
       <c r="F86" s="10"/>
       <c r="G86" s="10"/>
-      <c r="H86" s="10"/>
+      <c r="H86" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="I86" s="10" t="s">
         <v>11</v>
       </c>
@@ -3269,7 +3301,7 @@
       <c r="X87" s="6"/>
       <c r="Y87" s="6"/>
     </row>
-    <row r="88" spans="1:25" ht="12.75" customHeight="1">
+    <row r="88" spans="1:25" ht="50.25" customHeight="1">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8">
@@ -3279,13 +3311,17 @@
       <c r="E88" s="8"/>
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
+      <c r="H88" s="24">
+        <v>0</v>
+      </c>
       <c r="I88" s="10" t="s">
         <v>11</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
-      <c r="L88" s="10"/>
+      <c r="L88" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="M88" s="13"/>
       <c r="N88" s="6"/>
       <c r="O88" s="6"/>
@@ -3560,7 +3596,9 @@
       <c r="E97" s="8"/>
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
-      <c r="H97" s="10"/>
+      <c r="H97" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="I97" s="10" t="s">
         <v>11</v>
       </c>
@@ -3739,16 +3777,25 @@
       <c r="C106" s="8">
         <v>49</v>
       </c>
+      <c r="H106" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="I106" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:25">
+    <row r="107" spans="1:25" ht="38.25" customHeight="1">
       <c r="C107" s="8">
         <v>50</v>
       </c>
+      <c r="H107" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="I107" s="16" t="s">
         <v>11</v>
+      </c>
+      <c r="L107" s="26" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="1:25">
@@ -3824,6 +3871,9 @@
       <c r="C117" s="8">
         <v>60</v>
       </c>
+      <c r="H117" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="J117" s="16" t="s">
         <v>11</v>
       </c>
@@ -3888,6 +3938,9 @@
       <c r="C125" s="8">
         <v>68</v>
       </c>
+      <c r="H125" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="I125" s="16" t="s">
         <v>11</v>
       </c>
@@ -4282,7 +4335,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="177" spans="3:10">
+    <row r="177" spans="3:13">
       <c r="C177" s="8">
         <v>120</v>
       </c>
@@ -4290,15 +4343,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="3:10">
+    <row r="178" spans="3:13" ht="38.25">
       <c r="C178" s="8">
         <v>121</v>
       </c>
+      <c r="H178" s="27">
+        <v>0</v>
+      </c>
       <c r="J178" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="179" spans="3:10">
+      <c r="M178" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="179" spans="3:13">
       <c r="C179" s="8">
         <v>122</v>
       </c>
@@ -4306,7 +4365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="3:10">
+    <row r="180" spans="3:13">
       <c r="C180" s="8">
         <v>123</v>
       </c>
@@ -4314,7 +4373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="3:10">
+    <row r="181" spans="3:13">
       <c r="C181" s="8">
         <v>124</v>
       </c>
@@ -4322,7 +4381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="3:10">
+    <row r="182" spans="3:13">
       <c r="C182" s="8">
         <v>125</v>
       </c>
@@ -4330,7 +4389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="3:10">
+    <row r="183" spans="3:13">
       <c r="C183" s="8">
         <v>126</v>
       </c>
@@ -4338,7 +4397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="3:10">
+    <row r="184" spans="3:13">
       <c r="C184" s="8">
         <v>127</v>
       </c>
@@ -4346,7 +4405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="3:10">
+    <row r="185" spans="3:13">
       <c r="C185" s="8">
         <v>128</v>
       </c>
@@ -4354,7 +4413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="3:10">
+    <row r="186" spans="3:13">
       <c r="C186" s="8">
         <v>129</v>
       </c>
@@ -4362,7 +4421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="3:10">
+    <row r="187" spans="3:13">
       <c r="C187" s="8">
         <v>130</v>
       </c>
@@ -4373,7 +4432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="3:10">
+    <row r="188" spans="3:13">
       <c r="C188" s="8">
         <v>131</v>
       </c>
@@ -4381,7 +4440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="3:10">
+    <row r="189" spans="3:13">
       <c r="C189" s="8">
         <v>132</v>
       </c>
@@ -4389,12 +4448,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="3:10">
+    <row r="190" spans="3:13">
       <c r="C190" s="8">
         <v>133</v>
       </c>
     </row>
-    <row r="191" spans="3:10">
+    <row r="191" spans="3:13">
       <c r="C191" s="8">
         <v>134</v>
       </c>
@@ -4402,7 +4461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="3:10">
+    <row r="192" spans="3:13">
       <c r="C192" s="8">
         <v>135</v>
       </c>

</xml_diff>